<commit_message>
Add color data analyse
</commit_message>
<xml_diff>
--- a/Python-PIL/RGBA Werte.xlsx
+++ b/Python-PIL/RGBA Werte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\FLEDERWIND\FLEDERWIND\Python-PIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E649078-9F38-4492-9A1A-15A89A7D7B40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD90119E-5A25-437A-8061-E61FCF6ECBC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{BB5DA513-94CA-4C75-998B-606F1E368C73}"/>
   </bookViews>
@@ -141,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,6 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -471,7 +472,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,17 +501,17 @@
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
         <v>0</v>
       </c>
       <c r="E2" s="4">
-        <f t="shared" ref="E2:E34" si="0">AVERAGE(B2,C2,D2)</f>
+        <f t="shared" ref="E2:E33" si="0">AVERAGE(B2,C2,D2)</f>
         <v>0</v>
       </c>
       <c r="F2" s="7">
@@ -521,13 +522,13 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="8">
         <v>24</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="8">
         <v>24</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>0</v>
       </c>
       <c r="E3" s="4">
@@ -542,13 +543,13 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="8">
         <v>28</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="8">
         <v>28</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <v>0</v>
       </c>
       <c r="E4" s="4">
@@ -563,13 +564,13 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="8">
         <v>32</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
         <v>32</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="8">
         <v>0</v>
       </c>
       <c r="E5" s="4">
@@ -584,13 +585,13 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="8">
         <v>36</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="8">
         <v>36</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="8">
         <v>0</v>
       </c>
       <c r="E6" s="4">
@@ -605,13 +606,13 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="8">
         <v>40</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <v>40</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="8">
         <v>0</v>
       </c>
       <c r="E7" s="4">
@@ -626,13 +627,13 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="8">
         <v>43</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="8">
         <v>43</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="8">
         <v>0</v>
       </c>
       <c r="E8" s="4">
@@ -647,13 +648,13 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="8">
         <v>46</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="8">
         <v>46</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="8">
         <v>0</v>
       </c>
       <c r="E9" s="4">
@@ -668,13 +669,13 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="8">
         <v>49</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
         <v>49</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>0</v>
       </c>
       <c r="E10" s="4">
@@ -689,13 +690,13 @@
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="8">
         <v>52</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="8">
         <v>52</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="8">
         <v>0</v>
       </c>
       <c r="E11" s="4">
@@ -710,13 +711,13 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="8">
         <v>55</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="8">
         <v>55</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="8">
         <v>0</v>
       </c>
       <c r="E12" s="4">
@@ -731,13 +732,13 @@
       <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="8">
         <v>58</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="8">
         <v>58</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="8">
         <v>0</v>
       </c>
       <c r="E13" s="4">
@@ -752,13 +753,13 @@
       <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="8">
         <v>61</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="8">
         <v>61</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="8">
         <v>0</v>
       </c>
       <c r="E14" s="4">
@@ -773,13 +774,13 @@
       <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="8">
         <v>64</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="8">
         <v>64</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="8">
         <v>0</v>
       </c>
       <c r="E15" s="4">
@@ -794,13 +795,13 @@
       <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="8">
         <v>76</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="8">
         <v>76</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="8">
         <v>0</v>
       </c>
       <c r="E16" s="4">
@@ -815,13 +816,13 @@
       <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="8">
         <v>88</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="8">
         <v>88</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="8">
         <v>0</v>
       </c>
       <c r="E17" s="4">
@@ -836,13 +837,13 @@
       <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="8">
         <v>100</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="8">
         <v>100</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="8">
         <v>0</v>
       </c>
       <c r="E18" s="4">
@@ -857,13 +858,13 @@
       <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="8">
         <v>105</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="8">
         <v>105</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="8">
         <v>0</v>
       </c>
       <c r="E19" s="4">
@@ -878,13 +879,13 @@
       <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="8">
         <v>110</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="8">
         <v>110</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="8">
         <v>0</v>
       </c>
       <c r="E20" s="4">
@@ -899,13 +900,13 @@
       <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="8">
         <v>115</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="8">
         <v>115</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="8">
         <v>0</v>
       </c>
       <c r="E21" s="4">
@@ -920,13 +921,13 @@
       <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="8">
         <v>120</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="8">
         <v>120</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="8">
         <v>0</v>
       </c>
       <c r="E22" s="4">
@@ -941,13 +942,13 @@
       <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="8">
         <v>125</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="8">
         <v>125</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="8">
         <v>0</v>
       </c>
       <c r="E23" s="4">
@@ -962,13 +963,13 @@
       <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="8">
         <v>130</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="8">
         <v>130</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="8">
         <v>0</v>
       </c>
       <c r="E24" s="4">
@@ -983,13 +984,13 @@
       <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="8">
         <v>140</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="8">
         <v>140</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="8">
         <v>0</v>
       </c>
       <c r="E25" s="4">
@@ -1004,13 +1005,13 @@
       <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="8">
         <v>154</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="8">
         <v>154</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="8">
         <v>0</v>
       </c>
       <c r="E26" s="4">
@@ -1025,13 +1026,13 @@
       <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="8">
         <v>168</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="8">
         <v>168</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="8">
         <v>0</v>
       </c>
       <c r="E27" s="4">
@@ -1046,13 +1047,13 @@
       <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="8">
         <v>230</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="8">
         <v>230</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="8">
         <v>0</v>
       </c>
       <c r="E28" s="4">
@@ -1067,13 +1068,13 @@
       <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="8">
         <v>247</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="8">
         <v>247</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="8">
         <v>20</v>
       </c>
       <c r="E29" s="4">
@@ -1088,13 +1089,13 @@
       <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="8">
         <v>255</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="8">
         <v>255</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="8">
         <v>50</v>
       </c>
       <c r="E30" s="4">
@@ -1109,13 +1110,13 @@
       <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="8">
         <v>255</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="8">
         <v>255</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="8">
         <v>80</v>
       </c>
       <c r="E31" s="4">
@@ -1130,13 +1131,13 @@
       <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="8">
         <v>255</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="8">
         <v>255</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="8">
         <v>110</v>
       </c>
       <c r="E32" s="4">
@@ -1151,13 +1152,13 @@
       <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="8">
         <v>255</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="8">
         <v>255</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="8">
         <v>140</v>
       </c>
       <c r="E33" s="4">

</xml_diff>